<commit_message>
Add in decisions in diagrams
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/decision_1_v2.xlsx
+++ b/tests/integration_test_files/decision_1_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15F4B78-B42B-0A43-8EED-CBC1ADB74480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2F14D8-3F94-B545-9313-DCFF00117B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="5" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -5338,7 +5338,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixes for V2 exports
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/decision_1_v2.xlsx
+++ b/tests/integration_test_files/decision_1_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2F14D8-3F94-B545-9313-DCFF00117B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B68538C-80D3-AE40-84CF-9639B84F6A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="5" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="20840" yWindow="1920" windowWidth="33600" windowHeight="19460" firstSheet="5" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -1714,18 +1714,12 @@
     <t>label</t>
   </si>
   <si>
-    <t xml:space="preserve">from </t>
-  </si>
-  <si>
     <t>to</t>
   </si>
   <si>
     <t>timingValue</t>
   </si>
   <si>
-    <t>tofrom</t>
-  </si>
-  <si>
     <t>window</t>
   </si>
   <si>
@@ -1790,9 +1784,6 @@
   </si>
   <si>
     <t>FIXED</t>
-  </si>
-  <si>
-    <t>0..4 hours</t>
   </si>
   <si>
     <t>1 Day</t>
@@ -1854,6 +1845,15 @@
   <si>
     <t>DOSE: if major rash, 
 D14: If minor rash</t>
+  </si>
+  <si>
+    <t>-4..0 hours</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>toFrom</t>
   </si>
 </sst>
 </file>
@@ -2010,17 +2010,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3445,7 +3445,7 @@
         <v>207</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>195</v>
@@ -4995,23 +4995,23 @@
       <c r="A1" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -5028,76 +5028,76 @@
       <c r="A4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
@@ -5164,16 +5164,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5334,7 +5334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -5363,22 +5363,22 @@
         <v>471</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5395,16 +5395,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>219</v>
@@ -5421,7 +5421,7 @@
         <v>543</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -5430,10 +5430,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>219</v>
@@ -5445,59 +5445,59 @@
         <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="C5" s="17" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="C6" s="17" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="31" t="s">
-        <v>590</v>
+      <c r="H6" s="28" t="s">
+        <v>587</v>
       </c>
       <c r="I6" s="2"/>
     </row>
@@ -5505,7 +5505,7 @@
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="17" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -5527,7 +5527,7 @@
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="17" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>204</v>
@@ -5621,8 +5621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5E3869-2369-5644-A00D-6AA078FB1D13}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5647,155 +5647,155 @@
         <v>46</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>546</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>547</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B2" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="H2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>559</v>
+      </c>
+      <c r="B3" t="s">
+        <v>580</v>
+      </c>
+      <c r="C3" t="s">
+        <v>582</v>
+      </c>
+      <c r="D3" t="s">
+        <v>548</v>
+      </c>
+      <c r="E3" t="s">
+        <v>560</v>
+      </c>
+      <c r="F3" t="s">
         <v>561</v>
-      </c>
-      <c r="B3" t="s">
-        <v>583</v>
-      </c>
-      <c r="C3" t="s">
-        <v>585</v>
-      </c>
-      <c r="D3" t="s">
-        <v>550</v>
-      </c>
-      <c r="E3" t="s">
-        <v>562</v>
-      </c>
-      <c r="F3" t="s">
-        <v>563</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>560</v>
-      </c>
-      <c r="I3" t="s">
-        <v>570</v>
+        <v>558</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B4" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C4" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D4" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="G4" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B5" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C5" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D5" t="s">
+        <v>569</v>
+      </c>
+      <c r="E5" t="s">
+        <v>575</v>
+      </c>
+      <c r="F5" t="s">
+        <v>561</v>
+      </c>
+      <c r="G5" t="s">
         <v>572</v>
       </c>
-      <c r="E5" t="s">
-        <v>578</v>
-      </c>
-      <c r="F5" t="s">
-        <v>563</v>
-      </c>
-      <c r="G5" t="s">
-        <v>575</v>
-      </c>
       <c r="H5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C6" t="s">
         <v>219</v>
       </c>
       <c r="D6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="E6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="G6" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="H6" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>

</xml_diff>